<commit_message>
Abgabe Konzept in den Zeitplan eingebettet
</commit_message>
<xml_diff>
--- a/doc/01 Projektauftrag/Zeitplan.xlsx
+++ b/doc/01 Projektauftrag/Zeitplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30500" windowHeight="26900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Blatt1!$A$1:$CD$105</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Blatt1!$A$1:$CD$106</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="68">
   <si>
     <t>Vorgang</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>Fehler beheben</t>
+  </si>
+  <si>
+    <t>Abgabe Konzept</t>
   </si>
 </sst>
 </file>
@@ -304,8 +307,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="355">
+  <cellStyleXfs count="365">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -678,7 +691,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="355">
+  <cellStyles count="365">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -856,6 +869,11 @@
     <cellStyle name="Besuchter Link" xfId="350" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="352" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="364" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1033,9 +1051,14 @@
     <cellStyle name="Link" xfId="349" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="351" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="363" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1090,381 +1113,6 @@
       <border>
         <bottom style="thin">
           <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
         </bottom>
       </border>
     </dxf>
@@ -1823,13 +1471,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CE62"/>
+  <dimension ref="A1:CE63"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" colorId="55" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="AF15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="BK23" sqref="BK23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2481,6 +2129,12 @@
       <c r="AK14" t="s">
         <v>63</v>
       </c>
+      <c r="AL14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="1:83">
       <c r="B15" t="s">
@@ -2522,929 +2176,864 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:72">
-      <c r="A17" t="s">
+    <row r="17" spans="1:69">
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:69">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="AL17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AT17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AU17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AW17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AX17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AY17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AZ17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BA17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BB17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BC17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BD17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BE17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BF17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BG17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BH17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BI17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BJ17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BK17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BL17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BN17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BO17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BP17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BQ17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BR17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BS17" t="s">
-        <v>63</v>
-      </c>
-      <c r="BT17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:72">
-      <c r="B18" t="s">
+      <c r="AN18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AZ18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BC18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BD18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BE18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BG18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BI18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BJ18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BL18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BO18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BP18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BQ18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:69">
+      <c r="B19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:72">
-      <c r="C19" t="s">
+    <row r="20" spans="1:69">
+      <c r="C20" t="s">
         <v>56</v>
       </c>
-      <c r="AL19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:72">
-      <c r="B20" t="s">
+      <c r="AN20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:69">
+      <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="AL20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AT20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AU20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AW20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AX20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AY20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AZ20" t="s">
-        <v>63</v>
-      </c>
-      <c r="BA20" t="s">
-        <v>63</v>
-      </c>
-      <c r="BB20" t="s">
-        <v>63</v>
-      </c>
-      <c r="BC20" t="s">
-        <v>63</v>
-      </c>
-      <c r="BD20" t="s">
-        <v>63</v>
-      </c>
-      <c r="BE20" t="s">
-        <v>63</v>
-      </c>
-      <c r="BF20" t="s">
-        <v>63</v>
-      </c>
-      <c r="BG20" t="s">
-        <v>63</v>
-      </c>
-      <c r="BH20" t="s">
-        <v>63</v>
-      </c>
-      <c r="BI20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:72">
-      <c r="C21" t="s">
+      <c r="AN21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AZ21" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA21" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB21" t="s">
+        <v>63</v>
+      </c>
+      <c r="BC21" t="s">
+        <v>63</v>
+      </c>
+      <c r="BD21" t="s">
+        <v>63</v>
+      </c>
+      <c r="BE21" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF21" t="s">
+        <v>63</v>
+      </c>
+      <c r="BG21" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH21" t="s">
+        <v>63</v>
+      </c>
+      <c r="BI21" t="s">
+        <v>63</v>
+      </c>
+      <c r="BJ21" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:69">
+      <c r="C22" t="s">
         <v>54</v>
       </c>
-      <c r="AL21" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM21" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN21" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO21" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:72">
-      <c r="D22" t="s">
+      <c r="AN22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:69">
+      <c r="D23" t="s">
         <v>31</v>
       </c>
-      <c r="AL22" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:72">
-      <c r="D23" t="s">
+      <c r="AN23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:69">
+      <c r="D24" t="s">
         <v>47</v>
       </c>
-      <c r="AN23" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:72">
-      <c r="D24" t="s">
+      <c r="AP24" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:69">
+      <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="AP24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:72">
-      <c r="C25" t="s">
+      <c r="AR25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:69">
+      <c r="C26" t="s">
         <v>48</v>
       </c>
-      <c r="AQ25" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR25" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS25" t="s">
-        <v>63</v>
-      </c>
-      <c r="AT25" t="s">
-        <v>63</v>
-      </c>
-      <c r="AU25" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV25" t="s">
-        <v>63</v>
-      </c>
-      <c r="AW25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:72">
-      <c r="D26" t="s">
+      <c r="AS26" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT26" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU26" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV26" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW26" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX26" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:69">
+      <c r="D27" t="s">
         <v>52</v>
       </c>
-      <c r="AQ26" t="s">
-        <v>62</v>
-      </c>
-      <c r="AR26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:72">
-      <c r="D27" t="s">
+      <c r="AS27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:69">
+      <c r="D28" t="s">
         <v>21</v>
       </c>
-      <c r="AS27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:72">
-      <c r="D28" t="s">
+      <c r="AU28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:69">
+      <c r="D29" t="s">
         <v>50</v>
       </c>
-      <c r="AT28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:72">
-      <c r="D29" t="s">
+      <c r="AV29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:69">
+      <c r="D30" t="s">
         <v>49</v>
       </c>
-      <c r="AU29" t="s">
-        <v>62</v>
-      </c>
-      <c r="AV29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:72">
-      <c r="D30" t="s">
+      <c r="AW30" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:69">
+      <c r="D31" t="s">
         <v>51</v>
       </c>
-      <c r="AW30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:72">
-      <c r="C31" t="s">
+      <c r="AY31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:69">
+      <c r="C32" t="s">
         <v>25</v>
       </c>
-      <c r="AX31" t="s">
-        <v>63</v>
-      </c>
-      <c r="AY31" t="s">
-        <v>63</v>
-      </c>
-      <c r="AZ31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:72">
-      <c r="D32" t="s">
+      <c r="AZ32" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA32" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:63">
+      <c r="D33" t="s">
         <v>26</v>
       </c>
-      <c r="AX32" t="s">
-        <v>62</v>
-      </c>
-      <c r="AY32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="2:61">
-      <c r="D33" t="s">
+      <c r="AZ33" t="s">
+        <v>62</v>
+      </c>
+      <c r="BA33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="2:63">
+      <c r="D34" t="s">
         <v>27</v>
       </c>
-      <c r="AZ33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="2:61">
-      <c r="C34" t="s">
+      <c r="BB34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="2:63">
+      <c r="C35" t="s">
         <v>28</v>
       </c>
-      <c r="BA34" t="s">
-        <v>63</v>
-      </c>
-      <c r="BB34" t="s">
-        <v>63</v>
-      </c>
-      <c r="BC34" t="s">
-        <v>63</v>
-      </c>
-      <c r="BD34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="2:61">
-      <c r="D35" t="s">
+      <c r="BC35" t="s">
+        <v>63</v>
+      </c>
+      <c r="BD35" t="s">
+        <v>63</v>
+      </c>
+      <c r="BE35" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="2:63">
+      <c r="D36" t="s">
         <v>29</v>
       </c>
-      <c r="BA35" t="s">
-        <v>62</v>
-      </c>
-      <c r="BB35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="2:61">
-      <c r="D36" t="s">
+      <c r="BC36" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="2:63">
+      <c r="D37" t="s">
         <v>30</v>
       </c>
-      <c r="BC36" t="s">
-        <v>62</v>
-      </c>
-      <c r="BD36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="2:61">
-      <c r="C37" t="s">
+      <c r="BE37" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="2:63">
+      <c r="C38" t="s">
         <v>22</v>
       </c>
-      <c r="BE37" t="s">
-        <v>63</v>
-      </c>
-      <c r="BF37" t="s">
-        <v>63</v>
-      </c>
-      <c r="BG37" t="s">
-        <v>63</v>
-      </c>
-      <c r="BH37" t="s">
-        <v>63</v>
-      </c>
-      <c r="BI37" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="2:61">
-      <c r="D38" t="s">
+      <c r="BG38" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH38" t="s">
+        <v>63</v>
+      </c>
+      <c r="BI38" t="s">
+        <v>63</v>
+      </c>
+      <c r="BJ38" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="2:63">
+      <c r="D39" t="s">
         <v>23</v>
       </c>
-      <c r="BE38" t="s">
-        <v>62</v>
-      </c>
-      <c r="BF38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="2:61">
-      <c r="D39" t="s">
+      <c r="BG39" t="s">
+        <v>62</v>
+      </c>
+      <c r="BH39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="2:63">
+      <c r="D40" t="s">
         <v>24</v>
       </c>
-      <c r="BG39" t="s">
-        <v>62</v>
-      </c>
-      <c r="BH39" t="s">
-        <v>62</v>
-      </c>
-      <c r="BI39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="2:61">
-      <c r="B40" t="s">
+      <c r="BI40" t="s">
+        <v>62</v>
+      </c>
+      <c r="BJ40" t="s">
+        <v>62</v>
+      </c>
+      <c r="BK40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="2:63">
+      <c r="B41" t="s">
         <v>32</v>
       </c>
-      <c r="AL40" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM40" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN40" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO40" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP40" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ40" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR40" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS40" t="s">
-        <v>63</v>
-      </c>
-      <c r="AT40" t="s">
-        <v>63</v>
-      </c>
-      <c r="AU40" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="2:61">
-      <c r="C41" t="s">
+      <c r="AN41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="2:63">
+      <c r="C42" t="s">
         <v>33</v>
       </c>
-      <c r="AL41" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM41" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN41" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO41" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="2:61">
-      <c r="D42" t="s">
+      <c r="AN42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="2:63">
+      <c r="D43" t="s">
         <v>53</v>
       </c>
-      <c r="AL42" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM42" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN42" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO42" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP42" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="2:61">
-      <c r="C43" t="s">
+      <c r="AN43" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO43" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP43" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ43" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="2:63">
+      <c r="C44" t="s">
         <v>34</v>
       </c>
-      <c r="AQ43" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR43" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS43" t="s">
-        <v>63</v>
-      </c>
-      <c r="AT43" t="s">
-        <v>63</v>
-      </c>
-      <c r="AU43" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="44" spans="2:61">
-      <c r="D44" t="s">
+      <c r="AS44" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT44" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU44" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV44" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="2:63">
+      <c r="D45" t="s">
         <v>35</v>
       </c>
-      <c r="AQ44" t="s">
-        <v>62</v>
-      </c>
-      <c r="AR44" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="2:61">
-      <c r="D45" t="s">
+      <c r="AS45" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="2:63">
+      <c r="D46" t="s">
         <v>36</v>
       </c>
-      <c r="AS45" t="s">
-        <v>62</v>
-      </c>
-      <c r="AT45" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="2:61">
-      <c r="D46" t="s">
+      <c r="AU46" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="2:63">
+      <c r="D47" t="s">
         <v>37</v>
       </c>
-      <c r="AU46" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="2:61">
-      <c r="B47" t="s">
+      <c r="AW47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="2:63">
+      <c r="B48" t="s">
         <v>38</v>
       </c>
-      <c r="AV47" t="s">
-        <v>63</v>
-      </c>
-      <c r="AW47" t="s">
-        <v>63</v>
-      </c>
-      <c r="AX47" t="s">
-        <v>63</v>
-      </c>
-      <c r="AY47" t="s">
-        <v>63</v>
-      </c>
-      <c r="AZ47" t="s">
-        <v>63</v>
-      </c>
-      <c r="BA47" t="s">
-        <v>63</v>
-      </c>
-      <c r="BB47" t="s">
-        <v>63</v>
-      </c>
-      <c r="BC47" t="s">
-        <v>63</v>
-      </c>
-      <c r="BD47" t="s">
-        <v>63</v>
-      </c>
-      <c r="BE47" t="s">
-        <v>63</v>
-      </c>
-      <c r="BF47" t="s">
-        <v>63</v>
-      </c>
-      <c r="BG47" t="s">
-        <v>63</v>
-      </c>
-      <c r="BH47" t="s">
-        <v>63</v>
-      </c>
-      <c r="BI47" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="2:61">
-      <c r="C48" t="s">
+      <c r="AX48" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY48" t="s">
+        <v>63</v>
+      </c>
+      <c r="AZ48" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA48" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB48" t="s">
+        <v>63</v>
+      </c>
+      <c r="BC48" t="s">
+        <v>63</v>
+      </c>
+      <c r="BD48" t="s">
+        <v>63</v>
+      </c>
+      <c r="BE48" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF48" t="s">
+        <v>63</v>
+      </c>
+      <c r="BG48" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH48" t="s">
+        <v>63</v>
+      </c>
+      <c r="BI48" t="s">
+        <v>63</v>
+      </c>
+      <c r="BJ48" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:72">
+      <c r="C49" t="s">
         <v>39</v>
       </c>
-      <c r="AV48" t="s">
-        <v>63</v>
-      </c>
-      <c r="AW48" t="s">
-        <v>63</v>
-      </c>
-      <c r="AX48" t="s">
-        <v>63</v>
-      </c>
-      <c r="AY48" t="s">
-        <v>63</v>
-      </c>
-      <c r="AZ48" t="s">
-        <v>63</v>
-      </c>
-      <c r="BA48" t="s">
-        <v>63</v>
-      </c>
-      <c r="BB48" t="s">
-        <v>63</v>
-      </c>
-      <c r="BC48" t="s">
-        <v>63</v>
-      </c>
-      <c r="BD48" t="s">
-        <v>63</v>
-      </c>
-      <c r="BE48" t="s">
-        <v>63</v>
-      </c>
-      <c r="BF48" t="s">
-        <v>63</v>
-      </c>
-      <c r="BG48" t="s">
-        <v>63</v>
-      </c>
-      <c r="BH48" t="s">
-        <v>63</v>
-      </c>
-      <c r="BI48" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:77">
-      <c r="D49" t="s">
+      <c r="AX49" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY49" t="s">
+        <v>63</v>
+      </c>
+      <c r="AZ49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BC49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BD49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BE49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BG49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BI49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BJ49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:72">
+      <c r="D50" t="s">
         <v>40</v>
       </c>
-      <c r="AV49" t="s">
-        <v>62</v>
-      </c>
-      <c r="AW49" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:77">
-      <c r="D50" t="s">
+      <c r="AX50" t="s">
+        <v>62</v>
+      </c>
+      <c r="AY50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:72">
+      <c r="D51" t="s">
         <v>41</v>
       </c>
-      <c r="AX50" t="s">
-        <v>62</v>
-      </c>
-      <c r="AY50" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:77">
-      <c r="D51" t="s">
+      <c r="AZ51" t="s">
+        <v>62</v>
+      </c>
+      <c r="BA51" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:72">
+      <c r="D52" t="s">
         <v>57</v>
       </c>
-      <c r="AZ51" t="s">
-        <v>62</v>
-      </c>
-      <c r="BA51" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="52" spans="1:77">
-      <c r="C52" t="s">
+      <c r="BB52" t="s">
+        <v>62</v>
+      </c>
+      <c r="BC52" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:72">
+      <c r="C53" t="s">
         <v>42</v>
       </c>
-      <c r="BB52" t="s">
-        <v>63</v>
-      </c>
-      <c r="BC52" t="s">
-        <v>63</v>
-      </c>
-      <c r="BD52" t="s">
-        <v>63</v>
-      </c>
-      <c r="BE52" t="s">
-        <v>63</v>
-      </c>
-      <c r="BF52" t="s">
-        <v>63</v>
-      </c>
-      <c r="BG52" t="s">
-        <v>63</v>
-      </c>
-      <c r="BH52" t="s">
-        <v>63</v>
-      </c>
-      <c r="BI52" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="53" spans="1:77">
-      <c r="D53" t="s">
+      <c r="BD53" t="s">
+        <v>63</v>
+      </c>
+      <c r="BE53" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF53" t="s">
+        <v>63</v>
+      </c>
+      <c r="BG53" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH53" t="s">
+        <v>63</v>
+      </c>
+      <c r="BI53" t="s">
+        <v>63</v>
+      </c>
+      <c r="BJ53" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK53" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:72">
+      <c r="D54" t="s">
         <v>58</v>
       </c>
-      <c r="BB53" t="s">
-        <v>62</v>
-      </c>
-      <c r="BC53" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="54" spans="1:77">
-      <c r="D54" t="s">
+      <c r="BD54" t="s">
+        <v>62</v>
+      </c>
+      <c r="BE54" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:72">
+      <c r="D55" t="s">
         <v>59</v>
       </c>
-      <c r="BD54" t="s">
-        <v>62</v>
-      </c>
-      <c r="BE54" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:77">
-      <c r="D55" t="s">
+      <c r="BF55" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG55" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:72">
+      <c r="D56" t="s">
         <v>60</v>
       </c>
-      <c r="BF55" t="s">
-        <v>62</v>
-      </c>
-      <c r="BG55" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:77">
-      <c r="D56" t="s">
+      <c r="BH56" t="s">
+        <v>62</v>
+      </c>
+      <c r="BI56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:72">
+      <c r="D57" t="s">
         <v>43</v>
       </c>
-      <c r="BH56" t="s">
-        <v>62</v>
-      </c>
-      <c r="BI56" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="1:77">
-      <c r="B57" t="s">
+      <c r="BJ57" t="s">
+        <v>62</v>
+      </c>
+      <c r="BK57" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:72">
+      <c r="B58" t="s">
         <v>44</v>
       </c>
-      <c r="BJ57" t="s">
-        <v>63</v>
-      </c>
-      <c r="BK57" t="s">
-        <v>63</v>
-      </c>
-      <c r="BL57" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM57" t="s">
-        <v>63</v>
-      </c>
-      <c r="BN57" t="s">
-        <v>63</v>
-      </c>
-      <c r="BO57" t="s">
-        <v>63</v>
-      </c>
-      <c r="BP57" t="s">
-        <v>63</v>
-      </c>
-      <c r="BQ57" t="s">
-        <v>63</v>
-      </c>
-      <c r="BR57" t="s">
-        <v>63</v>
-      </c>
-      <c r="BS57" t="s">
-        <v>63</v>
-      </c>
-      <c r="BT57" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="58" spans="1:77">
-      <c r="C58" t="s">
+      <c r="BL58" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM58" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN58" t="s">
+        <v>63</v>
+      </c>
+      <c r="BO58" t="s">
+        <v>63</v>
+      </c>
+      <c r="BP58" t="s">
+        <v>63</v>
+      </c>
+      <c r="BQ58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:72">
+      <c r="C59" t="s">
         <v>64</v>
       </c>
-      <c r="BJ58" t="s">
-        <v>62</v>
-      </c>
-      <c r="BK58" t="s">
-        <v>62</v>
-      </c>
-      <c r="BL58" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:77">
-      <c r="C59" t="s">
+      <c r="BL59" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:72">
+      <c r="C60" t="s">
         <v>65</v>
       </c>
-      <c r="BM59" t="s">
-        <v>62</v>
-      </c>
-      <c r="BN59" t="s">
-        <v>62</v>
-      </c>
-      <c r="BO59" t="s">
-        <v>62</v>
-      </c>
-      <c r="BP59" t="s">
-        <v>62</v>
-      </c>
-      <c r="BQ59" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:77">
-      <c r="C60" t="s">
+      <c r="BN60" t="s">
+        <v>62</v>
+      </c>
+      <c r="BO60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:72">
+      <c r="C61" t="s">
         <v>66</v>
       </c>
-      <c r="BR60" t="s">
-        <v>62</v>
-      </c>
-      <c r="BS60" t="s">
-        <v>62</v>
-      </c>
-      <c r="BT60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61" spans="1:77">
-      <c r="A61" t="s">
+      <c r="BP61" t="s">
+        <v>62</v>
+      </c>
+      <c r="BQ61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:72">
+      <c r="A62" t="s">
         <v>16</v>
       </c>
-      <c r="BU61" t="s">
-        <v>63</v>
-      </c>
-      <c r="BV61" t="s">
-        <v>63</v>
-      </c>
-      <c r="BW61" t="s">
-        <v>63</v>
-      </c>
-      <c r="BX61" t="s">
-        <v>63</v>
-      </c>
-      <c r="BY61" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:77">
-      <c r="B62" t="s">
+      <c r="BR62" t="s">
+        <v>63</v>
+      </c>
+      <c r="BS62" t="s">
+        <v>63</v>
+      </c>
+      <c r="BT62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:72">
+      <c r="B63" t="s">
         <v>45</v>
       </c>
-      <c r="BU62" t="s">
-        <v>62</v>
-      </c>
-      <c r="BV62" t="s">
-        <v>62</v>
-      </c>
-      <c r="BW62" t="s">
-        <v>62</v>
-      </c>
-      <c r="BX62" t="s">
-        <v>62</v>
-      </c>
-      <c r="BY62" t="s">
+      <c r="BR63" t="s">
+        <v>62</v>
+      </c>
+      <c r="BS63" t="s">
+        <v>62</v>
+      </c>
+      <c r="BT63" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="W2:AA2"/>
-    <mergeCell ref="AB2:AF2"/>
-    <mergeCell ref="AG1:AK1"/>
-    <mergeCell ref="AL1:AP1"/>
-    <mergeCell ref="AQ1:AU1"/>
-    <mergeCell ref="AV1:AZ1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AF1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BK1:BO1"/>
-    <mergeCell ref="BP1:BT1"/>
-    <mergeCell ref="BU1:BY1"/>
     <mergeCell ref="BZ1:CD1"/>
     <mergeCell ref="AG2:AK2"/>
     <mergeCell ref="AL2:AP2"/>
@@ -3456,9 +3045,28 @@
     <mergeCell ref="BP2:BT2"/>
     <mergeCell ref="BU2:BY2"/>
     <mergeCell ref="BZ2:CD2"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BK1:BO1"/>
+    <mergeCell ref="BP1:BT1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="AG1:AK1"/>
+    <mergeCell ref="AL1:AP1"/>
+    <mergeCell ref="AQ1:AU1"/>
+    <mergeCell ref="AV1:AZ1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="R1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="AB2:AF2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="H4:CD106">
+  <conditionalFormatting sqref="H4:CD57 H64:CD107 BW58:CD61 H58:BR61 BX62:CD63 H62:BT63">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",H4)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Zeitplan und Pflichtenheft Update, letzteres in finaler Form
</commit_message>
<xml_diff>
--- a/doc/01 Projektauftrag/Zeitplan.xlsx
+++ b/doc/01 Projektauftrag/Zeitplan.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -225,7 +225,7 @@
     <t>Fehler beheben</t>
   </si>
   <si>
-    <t>Abgabe Konzept</t>
+    <t>Abgabe Fachkonzept</t>
   </si>
 </sst>
 </file>
@@ -1058,48 +1058,7 @@
     <cellStyle name="Link" xfId="363" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1473,11 +1432,11 @@
   </sheetPr>
   <dimension ref="A1:CE63"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" colorId="55" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="AF15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" defaultGridColor="0" colorId="55" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BK23" sqref="BK23"/>
+      <selection pane="bottomRight" activeCell="BU9" sqref="BU9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3076,7 +3035,7 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1" gridLines="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="8" scale="47" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="8" scale="48" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Zeitplan edited and added to Projektdokumentation
</commit_message>
<xml_diff>
--- a/doc/01 Projektauftrag/Zeitplan.xlsx
+++ b/doc/01 Projektauftrag/Zeitplan.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
+    <sheet name="Diagramm1" sheetId="2" r:id="rId1"/>
+    <sheet name="Blatt1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Blatt1!$A$1:$CI$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Blatt1!$A$1:$CI$67</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="80">
   <si>
     <t>Vorgang</t>
   </si>
@@ -264,6 +265,9 @@
   </si>
   <si>
     <t>Definitive Abnahme</t>
+  </si>
+  <si>
+    <t>PB</t>
   </si>
 </sst>
 </file>
@@ -1108,376 +1112,7 @@
     <cellStyle name="Link" xfId="363" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59999389629810485"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </left>
-        <right style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="hair">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1983,6 +1618,1554 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="400096960"/>
+        <c:axId val="400105976"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="400096960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="400105976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="400105976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="400096960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="175" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9301843" cy="6008914"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Gerade Verbindung mit Pfeil 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9169400" y="2616200"/>
+          <a:ext cx="3352800" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Gerade Verbindung mit Pfeil 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14871700" y="4089400"/>
+          <a:ext cx="749300" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Gerade Verbindung mit Pfeil 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14782800" y="4127500"/>
+          <a:ext cx="800100" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Gerade Verbindung mit Pfeil 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14859000" y="4140200"/>
+          <a:ext cx="723900" cy="7581900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Gerade Verbindung mit Pfeil 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15201900" y="4660900"/>
+          <a:ext cx="50800" cy="368300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Gerade Verbindung mit Pfeil 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15773400" y="6096000"/>
+          <a:ext cx="50800" cy="3225800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Gerade Verbindung mit Pfeil 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16370300" y="9296400"/>
+          <a:ext cx="0" cy="673100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Gerade Verbindung mit Pfeil 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15214600" y="4660900"/>
+          <a:ext cx="0" cy="1816100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>66</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Gerade Verbindung mit Pfeil 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16548100" y="7277100"/>
+          <a:ext cx="50800" cy="1828800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Gerade Verbindung mit Pfeil 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16941800" y="9156700"/>
+          <a:ext cx="12700" cy="1574800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Gerade Verbindung mit Pfeil 24"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15608300" y="5029200"/>
+          <a:ext cx="12700" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>70</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>75</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Gerade Verbindung mit Pfeil 26"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17335500" y="8699500"/>
+          <a:ext cx="977900" cy="4102100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>75</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>75</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Gerade Verbindung mit Pfeil 32"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18275300" y="11328400"/>
+          <a:ext cx="38100" cy="1422400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>66</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>66</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Gerade Verbindung mit Pfeil 34"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16598900" y="8128000"/>
+          <a:ext cx="12700" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>75</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Gerade Verbindung mit Pfeil 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16192500" y="12420600"/>
+          <a:ext cx="2108200" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>81</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>82</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Gerade Verbindung mit Pfeil 38"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19431000" y="13208000"/>
+          <a:ext cx="203200" cy="355600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-Design">
   <a:themeElements>
@@ -2310,11 +3493,11 @@
   </sheetPr>
   <dimension ref="A1:CN69"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" colorId="55" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="H13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" defaultGridColor="0" colorId="55" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="75" workbookViewId="0">
+      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BW52" sqref="BW52"/>
+      <selection pane="bottomRight" activeCell="BO57" sqref="BO57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3192,20 +4375,11 @@
       </c>
       <c r="F21" s="8">
         <f>COUNTIF(H21:CI21, "y")</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G21" t="s">
         <v>67</v>
       </c>
-      <c r="BC21" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD21" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="BE21" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="BF21" s="6" t="s">
         <v>50</v>
       </c>
@@ -3260,11 +4434,21 @@
       <c r="BW21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="BX21" s="6"/>
-      <c r="BY21" s="6"/>
-      <c r="BZ21" s="6"/>
-      <c r="CA21" s="6"/>
-      <c r="CB21" s="6"/>
+      <c r="BX21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="BY21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="BZ21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="CA21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="CB21" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="CC21" s="6"/>
       <c r="CD21" s="7"/>
       <c r="CE21" s="7"/>
@@ -3283,15 +4467,12 @@
         <v>60</v>
       </c>
       <c r="AM22" s="6"/>
-      <c r="BC22" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD22" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="BE22" s="6"/>
-      <c r="BF22" s="6"/>
-      <c r="BG22" s="6"/>
+      <c r="BF22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="BG22" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="BH22" s="6"/>
       <c r="BI22" s="6"/>
       <c r="BJ22" s="6"/>
@@ -3326,10 +4507,10 @@
         <f t="shared" ref="F23" si="1">COUNTIF(H23:CI23, "x")</f>
         <v>2</v>
       </c>
-      <c r="BC23" t="s">
-        <v>49</v>
-      </c>
-      <c r="BD23" t="s">
+      <c r="BF23" t="s">
+        <v>49</v>
+      </c>
+      <c r="BG23" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3344,10 +4525,10 @@
       <c r="G24" t="s">
         <v>59</v>
       </c>
-      <c r="BC24" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD24" t="s">
+      <c r="BH24" t="s">
+        <v>50</v>
+      </c>
+      <c r="BI24" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3359,10 +4540,10 @@
         <f t="shared" ref="F25" si="2">COUNTIF(H25:CI25, "x")</f>
         <v>2</v>
       </c>
-      <c r="BC25" t="s">
-        <v>49</v>
-      </c>
-      <c r="BD25" t="s">
+      <c r="BH25" t="s">
+        <v>49</v>
+      </c>
+      <c r="BI25" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3374,15 +4555,6 @@
         <f>COUNTIF(H26:CI26, "y")</f>
         <v>16</v>
       </c>
-      <c r="BC26" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD26" t="s">
-        <v>50</v>
-      </c>
-      <c r="BE26" t="s">
-        <v>50</v>
-      </c>
       <c r="BF26" t="s">
         <v>50</v>
       </c>
@@ -3420,6 +4592,15 @@
         <v>50</v>
       </c>
       <c r="BR26" t="s">
+        <v>50</v>
+      </c>
+      <c r="BS26" t="s">
+        <v>50</v>
+      </c>
+      <c r="BT26" t="s">
+        <v>50</v>
+      </c>
+      <c r="BU26" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3434,19 +4615,19 @@
       <c r="G27" t="s">
         <v>62</v>
       </c>
-      <c r="BC27" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD27" t="s">
-        <v>50</v>
-      </c>
-      <c r="BE27" t="s">
-        <v>50</v>
-      </c>
       <c r="BF27" t="s">
         <v>50</v>
       </c>
       <c r="BG27" t="s">
+        <v>50</v>
+      </c>
+      <c r="BH27" t="s">
+        <v>50</v>
+      </c>
+      <c r="BI27" t="s">
+        <v>50</v>
+      </c>
+      <c r="BJ27" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3458,10 +4639,10 @@
         <f t="shared" ref="F28:F30" si="3">COUNTIF(H28:CI28, "x")</f>
         <v>2</v>
       </c>
-      <c r="BC28" t="s">
-        <v>49</v>
-      </c>
-      <c r="BD28" t="s">
+      <c r="BF28" t="s">
+        <v>49</v>
+      </c>
+      <c r="BG28" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3473,10 +4654,10 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="BE29" t="s">
-        <v>49</v>
-      </c>
-      <c r="BF29" t="s">
+      <c r="BH29" t="s">
+        <v>49</v>
+      </c>
+      <c r="BI29" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3488,7 +4669,7 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="BG30" t="s">
+      <c r="BJ30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3500,14 +4681,8 @@
         <f>COUNTIF(H31:CI31, "y")</f>
         <v>7</v>
       </c>
-      <c r="BE31" t="s">
-        <v>50</v>
-      </c>
-      <c r="BF31" t="s">
-        <v>50</v>
-      </c>
-      <c r="BG31" t="s">
-        <v>50</v>
+      <c r="G31" t="s">
+        <v>79</v>
       </c>
       <c r="BH31" t="s">
         <v>50</v>
@@ -3519,6 +4694,15 @@
         <v>50</v>
       </c>
       <c r="BK31" t="s">
+        <v>50</v>
+      </c>
+      <c r="BL31" t="s">
+        <v>50</v>
+      </c>
+      <c r="BM31" t="s">
+        <v>50</v>
+      </c>
+      <c r="BN31" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3530,14 +4714,14 @@
         <f t="shared" ref="F32:F36" si="4">COUNTIF(H32:CI32, "x")</f>
         <v>2</v>
       </c>
-      <c r="BE32" t="s">
-        <v>49</v>
-      </c>
-      <c r="BF32" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BH32" t="s">
+        <v>49</v>
+      </c>
+      <c r="BI32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="2:74" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>19</v>
       </c>
@@ -3545,11 +4729,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="BG33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BJ33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="2:74" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>43</v>
       </c>
@@ -3557,11 +4741,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="BH34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BK34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="2:74" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>42</v>
       </c>
@@ -3569,14 +4753,14 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="BI35" t="s">
-        <v>49</v>
-      </c>
-      <c r="BJ35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BL35" t="s">
+        <v>49</v>
+      </c>
+      <c r="BM35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="2:74" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>44</v>
       </c>
@@ -3584,11 +4768,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="BK36" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BN36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="2:74" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>23</v>
       </c>
@@ -3596,23 +4780,26 @@
         <f>COUNTIF(H37:CI37, "y")</f>
         <v>5</v>
       </c>
-      <c r="BE37" t="s">
-        <v>50</v>
-      </c>
-      <c r="BF37" t="s">
-        <v>50</v>
-      </c>
-      <c r="BG37" t="s">
-        <v>50</v>
-      </c>
-      <c r="BH37" t="s">
-        <v>50</v>
-      </c>
-      <c r="BI37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ37" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK37" t="s">
+        <v>50</v>
+      </c>
+      <c r="BL37" t="s">
+        <v>50</v>
+      </c>
+      <c r="BM37" t="s">
+        <v>50</v>
+      </c>
+      <c r="BN37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="2:74" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>24</v>
       </c>
@@ -3620,14 +4807,14 @@
         <f t="shared" ref="F38:F40" si="5">COUNTIF(H38:CI38, "x")</f>
         <v>2</v>
       </c>
-      <c r="BE38" t="s">
-        <v>49</v>
-      </c>
-      <c r="BF38" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BJ38" t="s">
+        <v>49</v>
+      </c>
+      <c r="BK38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="2:74" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>25</v>
       </c>
@@ -3635,11 +4822,11 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="BG39" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BL39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="2:74" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>54</v>
       </c>
@@ -3647,14 +4834,14 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="BH40" t="s">
-        <v>49</v>
-      </c>
-      <c r="BI40" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BM40" t="s">
+        <v>49</v>
+      </c>
+      <c r="BN40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="2:74" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>26</v>
       </c>
@@ -3662,20 +4849,23 @@
         <f>COUNTIF(H41:CI41, "y")</f>
         <v>4</v>
       </c>
-      <c r="BL41" t="s">
-        <v>50</v>
-      </c>
-      <c r="BM41" t="s">
-        <v>50</v>
-      </c>
-      <c r="BN41" t="s">
-        <v>50</v>
+      <c r="G41" t="s">
+        <v>59</v>
       </c>
       <c r="BO41" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BP41" t="s">
+        <v>50</v>
+      </c>
+      <c r="BQ41" t="s">
+        <v>50</v>
+      </c>
+      <c r="BR41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="2:74" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>27</v>
       </c>
@@ -3683,14 +4873,14 @@
         <f t="shared" ref="F42:F43" si="6">COUNTIF(H42:CI42, "x")</f>
         <v>2</v>
       </c>
-      <c r="BL42" t="s">
-        <v>49</v>
-      </c>
-      <c r="BM42" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BO42" t="s">
+        <v>49</v>
+      </c>
+      <c r="BP42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="2:74" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>28</v>
       </c>
@@ -3698,23 +4888,20 @@
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="BN43" t="s">
-        <v>49</v>
-      </c>
-      <c r="BO43" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BQ43" t="s">
+        <v>49</v>
+      </c>
+      <c r="BR43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="2:74" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>20</v>
       </c>
       <c r="F44">
         <f>COUNTIF(H44:CI44, "y")</f>
-        <v>5</v>
-      </c>
-      <c r="BJ44" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="BK44" t="s">
         <v>50</v>
@@ -3728,8 +4915,14 @@
       <c r="BN44" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BO44" t="s">
+        <v>50</v>
+      </c>
+      <c r="BP44" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="2:74" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>21</v>
       </c>
@@ -3737,14 +4930,17 @@
         <f t="shared" ref="F45:F46" si="7">COUNTIF(H45:CI45, "x")</f>
         <v>2</v>
       </c>
-      <c r="BJ45" t="s">
-        <v>49</v>
-      </c>
-      <c r="BK45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO45" t="s">
+        <v>49</v>
+      </c>
+      <c r="BP45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="2:74" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>22</v>
       </c>
@@ -3752,17 +4948,20 @@
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
+      <c r="G46" t="s">
+        <v>62</v>
+      </c>
+      <c r="BK46" t="s">
+        <v>49</v>
+      </c>
       <c r="BL46" t="s">
         <v>49</v>
       </c>
       <c r="BM46" t="s">
         <v>49</v>
       </c>
-      <c r="BN46" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="2:70" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>30</v>
       </c>
@@ -3770,18 +4969,6 @@
         <f>COUNTIF(H47:CI47, "y")</f>
         <v>9</v>
       </c>
-      <c r="BJ47" t="s">
-        <v>50</v>
-      </c>
-      <c r="BK47" t="s">
-        <v>50</v>
-      </c>
-      <c r="BL47" t="s">
-        <v>50</v>
-      </c>
-      <c r="BM47" t="s">
-        <v>50</v>
-      </c>
       <c r="BN47" t="s">
         <v>50</v>
       </c>
@@ -3797,8 +4984,20 @@
       <c r="BR47" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="BS47" t="s">
+        <v>50</v>
+      </c>
+      <c r="BT47" t="s">
+        <v>50</v>
+      </c>
+      <c r="BU47" t="s">
+        <v>50</v>
+      </c>
+      <c r="BV47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="2:74" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>31</v>
       </c>
@@ -3806,17 +5005,8 @@
         <f>COUNTIF(H48:CI48, "y")</f>
         <v>9</v>
       </c>
-      <c r="BJ48" t="s">
-        <v>50</v>
-      </c>
-      <c r="BK48" t="s">
-        <v>50</v>
-      </c>
-      <c r="BL48" t="s">
-        <v>50</v>
-      </c>
-      <c r="BM48" t="s">
-        <v>50</v>
+      <c r="G48" t="s">
+        <v>62</v>
       </c>
       <c r="BN48" t="s">
         <v>50</v>
@@ -3833,8 +5023,20 @@
       <c r="BR48" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BS48" t="s">
+        <v>50</v>
+      </c>
+      <c r="BT48" t="s">
+        <v>50</v>
+      </c>
+      <c r="BU48" t="s">
+        <v>50</v>
+      </c>
+      <c r="BV48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="2:81" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>68</v>
       </c>
@@ -3842,23 +5044,23 @@
         <f t="shared" ref="F49" si="8">COUNTIF(H49:CI49, "x")</f>
         <v>5</v>
       </c>
-      <c r="BJ49" t="s">
-        <v>49</v>
-      </c>
-      <c r="BK49" t="s">
-        <v>49</v>
-      </c>
-      <c r="BL49" t="s">
-        <v>49</v>
-      </c>
-      <c r="BM49" t="s">
-        <v>49</v>
-      </c>
       <c r="BN49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BO49" t="s">
+        <v>49</v>
+      </c>
+      <c r="BP49" t="s">
+        <v>49</v>
+      </c>
+      <c r="BQ49" t="s">
+        <v>49</v>
+      </c>
+      <c r="BR49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="2:81" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>69</v>
       </c>
@@ -3866,14 +5068,14 @@
         <f t="shared" ref="F50:F56" si="9">COUNTIF(H50:CI50, "x")</f>
         <v>2</v>
       </c>
-      <c r="BO50" t="s">
-        <v>49</v>
-      </c>
-      <c r="BP50" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BS50" t="s">
+        <v>49</v>
+      </c>
+      <c r="BT50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="2:81" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>70</v>
       </c>
@@ -3881,14 +5083,14 @@
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="BQ51" t="s">
-        <v>49</v>
-      </c>
-      <c r="BR51" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BU51" t="s">
+        <v>49</v>
+      </c>
+      <c r="BV51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="2:81" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>32</v>
       </c>
@@ -3896,29 +5098,32 @@
         <f>COUNTIF(H52:CI52, "y")</f>
         <v>7</v>
       </c>
-      <c r="BJ52" t="s">
-        <v>50</v>
-      </c>
-      <c r="BK52" t="s">
-        <v>50</v>
-      </c>
-      <c r="BL52" t="s">
-        <v>50</v>
-      </c>
-      <c r="BM52" t="s">
-        <v>50</v>
-      </c>
-      <c r="BN52" t="s">
-        <v>50</v>
-      </c>
-      <c r="BO52" t="s">
-        <v>50</v>
-      </c>
-      <c r="BP52" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ52" t="s">
+        <v>50</v>
+      </c>
+      <c r="BR52" t="s">
+        <v>50</v>
+      </c>
+      <c r="BS52" t="s">
+        <v>50</v>
+      </c>
+      <c r="BT52" t="s">
+        <v>50</v>
+      </c>
+      <c r="BU52" t="s">
+        <v>50</v>
+      </c>
+      <c r="BV52" t="s">
+        <v>50</v>
+      </c>
+      <c r="BW52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="2:81" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
         <v>33</v>
       </c>
@@ -3926,14 +5131,14 @@
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="BJ53" t="s">
-        <v>49</v>
-      </c>
-      <c r="BK53" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="54" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BQ53" t="s">
+        <v>49</v>
+      </c>
+      <c r="BR53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="2:81" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
         <v>34</v>
       </c>
@@ -3941,14 +5146,14 @@
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="BL54" t="s">
-        <v>49</v>
-      </c>
-      <c r="BM54" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BS54" t="s">
+        <v>49</v>
+      </c>
+      <c r="BT54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="2:81" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>71</v>
       </c>
@@ -3956,14 +5161,14 @@
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="BN55" t="s">
-        <v>49</v>
-      </c>
-      <c r="BO55" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BU55" t="s">
+        <v>49</v>
+      </c>
+      <c r="BV55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="2:81" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>35</v>
       </c>
@@ -3971,11 +5176,11 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="BP56" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="57" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BW56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="2:81" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>36</v>
       </c>
@@ -3986,15 +5191,6 @@
       <c r="G57" t="s">
         <v>63</v>
       </c>
-      <c r="BC57" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD57" t="s">
-        <v>50</v>
-      </c>
-      <c r="BE57" t="s">
-        <v>50</v>
-      </c>
       <c r="BF57" t="s">
         <v>50</v>
       </c>
@@ -4007,8 +5203,17 @@
       <c r="BI57" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="58" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BJ57" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK57" t="s">
+        <v>50</v>
+      </c>
+      <c r="BL57" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="2:81" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>72</v>
       </c>
@@ -4016,14 +5221,14 @@
         <f t="shared" ref="F58:F61" si="10">COUNTIF(H58:CI58, "x")</f>
         <v>2</v>
       </c>
-      <c r="BC58" t="s">
-        <v>49</v>
-      </c>
-      <c r="BD58" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BF58" t="s">
+        <v>49</v>
+      </c>
+      <c r="BG58" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="2:81" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>73</v>
       </c>
@@ -4031,14 +5236,14 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="BE59" t="s">
-        <v>49</v>
-      </c>
-      <c r="BF59" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="60" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BH59" t="s">
+        <v>49</v>
+      </c>
+      <c r="BI59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="2:81" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>74</v>
       </c>
@@ -4046,14 +5251,14 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="BG60" t="s">
-        <v>49</v>
-      </c>
-      <c r="BH60" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="61" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BJ60" t="s">
+        <v>49</v>
+      </c>
+      <c r="BK60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="2:81" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>37</v>
       </c>
@@ -4061,11 +5266,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="BI61" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="62" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BL61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="2:81" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>38</v>
       </c>
@@ -4073,26 +5278,29 @@
         <f>COUNTIF(H62:CI62, "y")</f>
         <v>6</v>
       </c>
-      <c r="BS62" t="s">
-        <v>50</v>
-      </c>
-      <c r="BT62" t="s">
-        <v>50</v>
-      </c>
-      <c r="BU62" t="s">
-        <v>50</v>
-      </c>
-      <c r="BV62" t="s">
-        <v>50</v>
-      </c>
-      <c r="BW62" t="s">
-        <v>50</v>
+      <c r="G62" t="s">
+        <v>67</v>
       </c>
       <c r="BX62" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="63" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BY62" t="s">
+        <v>50</v>
+      </c>
+      <c r="BZ62" t="s">
+        <v>50</v>
+      </c>
+      <c r="CA62" t="s">
+        <v>50</v>
+      </c>
+      <c r="CB62" t="s">
+        <v>50</v>
+      </c>
+      <c r="CC62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="2:81" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>51</v>
       </c>
@@ -4100,14 +5308,14 @@
         <f t="shared" ref="F63:F65" si="11">COUNTIF(H63:CI63, "x")</f>
         <v>2</v>
       </c>
-      <c r="BS63" t="s">
-        <v>49</v>
-      </c>
-      <c r="BT63" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="64" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BX63" t="s">
+        <v>49</v>
+      </c>
+      <c r="BY63" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="2:81" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>52</v>
       </c>
@@ -4115,10 +5323,10 @@
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="BU64" t="s">
-        <v>49</v>
-      </c>
-      <c r="BV64" t="s">
+      <c r="BZ64" t="s">
+        <v>49</v>
+      </c>
+      <c r="CA64" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4130,10 +5338,10 @@
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="BW65" t="s">
-        <v>49</v>
-      </c>
-      <c r="BX65" t="s">
+      <c r="CB65" t="s">
+        <v>49</v>
+      </c>
+      <c r="CC65" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4229,6 +5437,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="BP1:BT1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="BZ1:CD1"/>
+    <mergeCell ref="AG2:AK2"/>
+    <mergeCell ref="AL2:AP2"/>
+    <mergeCell ref="AQ2:AU2"/>
+    <mergeCell ref="AV2:AZ2"/>
+    <mergeCell ref="BA2:BE2"/>
+    <mergeCell ref="BF2:BJ2"/>
+    <mergeCell ref="BK2:BO2"/>
+    <mergeCell ref="BP2:BT2"/>
+    <mergeCell ref="BU2:BY2"/>
+    <mergeCell ref="BZ2:CD2"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BK1:BO1"/>
     <mergeCell ref="CJ1:CN1"/>
     <mergeCell ref="CJ2:CN2"/>
     <mergeCell ref="CE2:CI2"/>
@@ -4245,93 +5471,92 @@
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="R1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AF1"/>
-    <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="AG2:AK2"/>
-    <mergeCell ref="AL2:AP2"/>
-    <mergeCell ref="AQ2:AU2"/>
-    <mergeCell ref="AV2:AZ2"/>
-    <mergeCell ref="BA2:BE2"/>
-    <mergeCell ref="BF2:BJ2"/>
-    <mergeCell ref="BK2:BO2"/>
-    <mergeCell ref="BP2:BT2"/>
-    <mergeCell ref="BU2:BY2"/>
-    <mergeCell ref="BZ2:CD2"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BK1:BO1"/>
-    <mergeCell ref="BP1:BT1"/>
-    <mergeCell ref="BU1:BY1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="H68:CD111 H4:CD13 H15:AA20 AN15:AS20 CH23:CM58 BV22:CM22 BM66:CC66 BM67:BZ67 CE66:CG67 H21:CG21 CA58:CC58 H22:AM67 BC62:BL67 BC60:BD61 BE59:BH60 CA63:CA65 BC22:BD22 BC23:CC30 AT15:BE16 AT18:BE20 AT17:BD17 BF18 CH66:CN66 BG15:BI20 BL14:CD20 H14:BI14 BJ58:BL61 BT58 BC58:BI58 BT59:CC61 BI59:BI61 BT57:CC57 BC57:BL57 BJ47:CC51 BC37:BD40 BO31:CC36 BC31:BK36 BH40:BI40 BT37:CC40 BE37:BI39 BJ37:BN40 BE40:BF40 BC41:BK43 BL42:BQ43 BX41:CC43 BL41:BS41 BT44:BW46 CC44:CC46 BC44:BQ46 BV52:CC56 BJ52:BP56 BZ62:CA62 BM62:BX65">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="x">
+  <conditionalFormatting sqref="H68:CD111 H4:CD13 H15:AA20 AN15:AS20 CH23:CM58 BM66:CC66 BM67:BZ67 CE66:CG67 H22:AM67 BF60:BG61 BH59:BK60 BF22:BG22 BF23:CB23 AT15:BE16 AT18:BE20 AT17:BD17 BF18 CH66:CN66 BG15:BI20 BL14:CD20 H14:BI14 BM58:BO61 BW58 BF58:BL58 BL59:BL61 BW57:CB57 BF57:BO57 BF37:BG40 BR31:CB36 BF31:BN36 BM40:BN40 BW37:CB40 BJ37:BN39 BO37:BQ40 BJ40:BK40 CA41:CB43 BO41:BV41 BW44:BZ46 BY52:CB56 BQ52:BW56 BF26:CB30 BH24:CB25 BF41:BN43 BF44:BL45 BR46:BT46 BO42:BT43 BO45:BT45 BP44:BT44 BN44 BF46:BM46 BN47:CB51 CC23:CC61 BY22:CM22 H21:BB21 BF21:CG21 BC66:BL67 BF62:BU65 BW59:CB61 BX62:CC65">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE17">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",BE17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",BE17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CH67">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",CH67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",CH67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CI67">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",CI67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",CI67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ68">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",CJ68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",CJ68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CK68">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",CK68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",CK68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL69">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",CL69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",CL69)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM69">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",CM69)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="y">
+      <formula>NOT(ISERROR(SEARCH("y",CM69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM44">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH("x",BM44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="y">
+      <formula>NOT(ISERROR(SEARCH("y",BM44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BO44">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH("x",BO44)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="y">
-      <formula>NOT(ISERROR(SEARCH("y",CM69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("y",BO44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1" gridLines="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.5" footer="0.5"/>
   <pageSetup paperSize="8" scale="69" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>